<commit_message>
Updated test cases & test plan
</commit_message>
<xml_diff>
--- a/Test Plan/Test Plan SauceDemo.xlsx
+++ b/Test Plan/Test Plan SauceDemo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhase\Desktop\Capstone Project\Test Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhase\eclipse-workspace\Capstone_Project_SauceDemo_Testing\Test Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDA48E5-53BC-4955-8277-E25C303A286D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFF5F55-73D9-450D-9986-92A0EBF86646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="79">
   <si>
     <t>Module Name</t>
   </si>
@@ -223,19 +223,40 @@
     <t>- Checkout complete confirmation message</t>
   </si>
   <si>
-    <t>Logout</t>
-  </si>
-  <si>
-    <t>Logout button, Navigation to login</t>
-  </si>
-  <si>
-    <t>Session timeout, Force logout</t>
-  </si>
-  <si>
-    <t>Pass if logout redirects to login, session ends, and no access to authenticated pages</t>
-  </si>
-  <si>
-    <t>Testing paused if logout button fails or user session persists</t>
+    <t>Menu Navigation</t>
+  </si>
+  <si>
+    <t>- Verify All Items navigates to inventory page</t>
+  </si>
+  <si>
+    <t>- Verify About opens https://saucelabs.com/</t>
+  </si>
+  <si>
+    <t>- Verify Logout redirects to login page</t>
+  </si>
+  <si>
+    <t>- Verify Reset App State clears cart</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>All menu buttons work as expected:</t>
+  </si>
+  <si>
+    <t>- All Items on inventory page</t>
+  </si>
+  <si>
+    <t>- About page opens external site</t>
+  </si>
+  <si>
+    <t>- Logout redirects to login</t>
+  </si>
+  <si>
+    <t>- Reset App clears cart</t>
+  </si>
+  <si>
+    <t>Any failure of menu navigation buttons</t>
   </si>
 </sst>
 </file>
@@ -286,7 +307,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -623,47 +644,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -710,6 +690,75 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -719,6 +768,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -731,84 +783,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1111,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1188,202 +1166,202 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="35">
+      <c r="A3" s="43">
         <v>1</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="37" t="s">
+      <c r="K3" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="L3" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="27"/>
-      <c r="B4" s="24"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="39"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="22"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="27"/>
-      <c r="B5" s="24"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="39"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="22"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="27"/>
-      <c r="B6" s="24"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="39"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="22"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
-      <c r="B7" s="24"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="39"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="22"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
-      <c r="B8" s="24"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="39"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="22"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="39"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="22"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="27"/>
-      <c r="B10" s="24"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="39"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="22"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
-      <c r="B11" s="24"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="39"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="22"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="27"/>
-      <c r="B12" s="24"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="39"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="22"/>
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="27"/>
-      <c r="B13" s="24"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="40"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="23"/>
     </row>
     <row r="14" spans="1:12" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="16">
@@ -1424,374 +1402,472 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="38">
+      <c r="A15" s="21">
         <v>3</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="21" t="s">
         <v>48</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="38" t="s">
+      <c r="F15" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="38" t="s">
+      <c r="H15" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="38" t="s">
+      <c r="I15" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="44" t="s">
+      <c r="J15" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="K15" s="44" t="s">
+      <c r="K15" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="L15" s="38" t="s">
+      <c r="L15" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
-      <c r="B16" s="39"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="39"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="22"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="39"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="22"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="39"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="22"/>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="40"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="23"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="38">
+      <c r="A20" s="21">
         <v>4</v>
       </c>
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="27" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="36" t="s">
+      <c r="E20" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="36" t="s">
+      <c r="F20" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="36" t="s">
+      <c r="G20" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="H20" s="36" t="s">
+      <c r="H20" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="36" t="s">
+      <c r="I20" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J20" s="36" t="s">
+      <c r="J20" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K20" s="37" t="s">
+      <c r="K20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="L20" s="38" t="s">
+      <c r="L20" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="39"/>
-      <c r="B21" s="42"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="28"/>
       <c r="C21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="39"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="22"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="39"/>
-      <c r="B22" s="42"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="28"/>
       <c r="C22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="39"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="22"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="39"/>
-      <c r="B23" s="42"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="39"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="22"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="39"/>
-      <c r="B24" s="42"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="39"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="22"/>
     </row>
     <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="40"/>
-      <c r="B25" s="43"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="40"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="23"/>
     </row>
     <row r="26" spans="1:12" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="26">
+      <c r="A26" s="33">
         <v>5</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="36" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="D26" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="F26" s="23" t="s">
+      <c r="F26" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="23" t="s">
+      <c r="G26" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="H26" s="17" t="s">
+      <c r="H26" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="23" t="s">
+      <c r="I26" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="J26" s="17" t="s">
+      <c r="J26" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="K26" s="17" t="s">
+      <c r="K26" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="L26" s="20" t="s">
+      <c r="L26" s="44" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="27"/>
-      <c r="B27" s="30"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="33"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="21"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="45"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="27"/>
-      <c r="B28" s="30"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="33"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="21"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="41"/>
+      <c r="L28" s="45"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="27"/>
-      <c r="B29" s="30"/>
+      <c r="A29" s="34"/>
+      <c r="B29" s="31"/>
       <c r="C29" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="33"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="21"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="41"/>
+      <c r="L29" s="45"/>
     </row>
     <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="28"/>
-      <c r="B30" s="31"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="32"/>
       <c r="C30" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="34"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="22"/>
-    </row>
-    <row r="31" spans="1:12" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="47">
+      <c r="D30" s="39"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="46"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="33">
         <v>6</v>
       </c>
-      <c r="B31" s="48" t="s">
+      <c r="B31" s="47" t="s">
         <v>67</v>
       </c>
       <c r="C31" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="48" t="s">
+      <c r="D31" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="H31" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="K31" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="L31" s="44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="34"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="E31" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" s="48" t="s">
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="45"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="34"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G31" s="48" t="s">
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="45"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="34"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H31" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="I31" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="J31" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="K31" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="L31" s="49" t="s">
-        <v>12</v>
-      </c>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="45"/>
+    </row>
+    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="35"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
+      <c r="L35" s="46"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="K15:K19"/>
-    <mergeCell ref="L15:L19"/>
-    <mergeCell ref="E15:E19"/>
-    <mergeCell ref="F15:F19"/>
-    <mergeCell ref="G15:G19"/>
-    <mergeCell ref="H15:H19"/>
-    <mergeCell ref="I15:I19"/>
+  <mergeCells count="54">
+    <mergeCell ref="H31:H35"/>
+    <mergeCell ref="I31:I35"/>
+    <mergeCell ref="J31:J35"/>
+    <mergeCell ref="K31:K35"/>
+    <mergeCell ref="L31:L35"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="D31:D35"/>
+    <mergeCell ref="E31:E35"/>
+    <mergeCell ref="G31:G35"/>
+    <mergeCell ref="K26:K30"/>
+    <mergeCell ref="L26:L30"/>
+    <mergeCell ref="F26:F30"/>
+    <mergeCell ref="G26:G30"/>
+    <mergeCell ref="H26:H30"/>
+    <mergeCell ref="I26:I30"/>
+    <mergeCell ref="J26:J30"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="E26:E30"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="D3:D13"/>
+    <mergeCell ref="B3:B13"/>
+    <mergeCell ref="E3:E13"/>
+    <mergeCell ref="E20:E25"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="K20:K25"/>
+    <mergeCell ref="L20:L25"/>
+    <mergeCell ref="F3:F13"/>
+    <mergeCell ref="K3:K13"/>
+    <mergeCell ref="L3:L13"/>
+    <mergeCell ref="G3:G13"/>
+    <mergeCell ref="H3:H13"/>
     <mergeCell ref="F20:F25"/>
     <mergeCell ref="G20:G25"/>
     <mergeCell ref="I3:I13"/>
@@ -1804,31 +1880,13 @@
     <mergeCell ref="H20:H25"/>
     <mergeCell ref="I20:I25"/>
     <mergeCell ref="J20:J25"/>
-    <mergeCell ref="K20:K25"/>
-    <mergeCell ref="L20:L25"/>
-    <mergeCell ref="F3:F13"/>
-    <mergeCell ref="K3:K13"/>
-    <mergeCell ref="L3:L13"/>
-    <mergeCell ref="G3:G13"/>
-    <mergeCell ref="H3:H13"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="E26:E30"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="D3:D13"/>
-    <mergeCell ref="B3:B13"/>
-    <mergeCell ref="E3:E13"/>
-    <mergeCell ref="E20:E25"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="K26:K30"/>
-    <mergeCell ref="L26:L30"/>
-    <mergeCell ref="F26:F30"/>
-    <mergeCell ref="G26:G30"/>
-    <mergeCell ref="H26:H30"/>
-    <mergeCell ref="I26:I30"/>
-    <mergeCell ref="J26:J30"/>
+    <mergeCell ref="K15:K19"/>
+    <mergeCell ref="L15:L19"/>
+    <mergeCell ref="E15:E19"/>
+    <mergeCell ref="F15:F19"/>
+    <mergeCell ref="G15:G19"/>
+    <mergeCell ref="H15:H19"/>
+    <mergeCell ref="I15:I19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>